<commit_message>
Added variable "index" to test
</commit_message>
<xml_diff>
--- a/tests/Templates/4.xlsx
+++ b/tests/Templates/4.xlsx
@@ -10,16 +10,16 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dates">Лист1!$F$3</definedName>
-    <definedName name="PlanData">Лист1!$A$4:$G$5</definedName>
-    <definedName name="PlanData_Hours">Лист1!$F$4</definedName>
+    <definedName name="dates">Лист1!$G$3</definedName>
+    <definedName name="PlanData">Лист1!$A$4:$H$5</definedName>
+    <definedName name="PlanData_Hours">Лист1!$G$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>&amp;=SUM(PlanData_Hours)&lt;&lt;OnlyValues&gt;&gt;</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>{{index+1}}</t>
   </si>
 </sst>
 </file>
@@ -498,98 +504,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="2" max="7" width="11.33203125" customWidth="1"/>
+    <col min="2" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="F1" s="10" t="s">
+    <row r="1" spans="1:11">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K1" s="10"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="D5" s="3"/>
+    <row r="5" spans="1:11">
       <c r="E5" s="3"/>
-      <c r="H5">
+      <c r="F5" s="3"/>
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>11</v>
       </c>
@@ -611,17 +623,17 @@
       <c r="G6">
         <v>17</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>12</v>
       </c>
@@ -643,17 +655,17 @@
       <c r="G7">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>13</v>
       </c>
@@ -675,17 +687,17 @@
       <c r="G8">
         <v>19</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>6</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>7</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>14</v>
       </c>
@@ -707,17 +719,17 @@
       <c r="G9">
         <v>20</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>7</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>8</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>15</v>
       </c>
@@ -740,7 +752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>16</v>
       </c>
@@ -765,7 +777,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added variable "index" to test (#78)
</commit_message>
<xml_diff>
--- a/tests/Templates/4.xlsx
+++ b/tests/Templates/4.xlsx
@@ -10,16 +10,16 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dates">Лист1!$F$3</definedName>
-    <definedName name="PlanData">Лист1!$A$4:$G$5</definedName>
-    <definedName name="PlanData_Hours">Лист1!$F$4</definedName>
+    <definedName name="dates">Лист1!$G$3</definedName>
+    <definedName name="PlanData">Лист1!$A$4:$H$5</definedName>
+    <definedName name="PlanData_Hours">Лист1!$G$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>&amp;=SUM(PlanData_Hours)&lt;&lt;OnlyValues&gt;&gt;</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>{{index+1}}</t>
   </si>
 </sst>
 </file>
@@ -498,98 +504,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="2" max="7" width="11.33203125" customWidth="1"/>
+    <col min="2" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="F1" s="10" t="s">
+    <row r="1" spans="1:11">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K1" s="10"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="D5" s="3"/>
+    <row r="5" spans="1:11">
       <c r="E5" s="3"/>
-      <c r="H5">
+      <c r="F5" s="3"/>
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>11</v>
       </c>
@@ -611,17 +623,17 @@
       <c r="G6">
         <v>17</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>12</v>
       </c>
@@ -643,17 +655,17 @@
       <c r="G7">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>13</v>
       </c>
@@ -675,17 +687,17 @@
       <c r="G8">
         <v>19</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>6</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>7</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>14</v>
       </c>
@@ -707,17 +719,17 @@
       <c r="G9">
         <v>20</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>7</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>8</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>15</v>
       </c>
@@ -740,7 +752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>16</v>
       </c>
@@ -765,7 +777,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added hyperlynk test examples
</commit_message>
<xml_diff>
--- a/tests/Templates/4.xlsx
+++ b/tests/Templates/4.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\asr\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
@@ -10,16 +15,16 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dates">Лист1!$G$3</definedName>
-    <definedName name="PlanData">Лист1!$A$4:$H$5</definedName>
-    <definedName name="PlanData_Hours">Лист1!$G$4</definedName>
+    <definedName name="dates">Лист1!$H$3</definedName>
+    <definedName name="PlanData">Лист1!$A$4:$I$5</definedName>
+    <definedName name="PlanData_Hours">Лист1!$H$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -61,16 +66,22 @@
   </si>
   <si>
     <t>{{index+1}}</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>&amp;=HYPERLINK("mailto:{{item.Email}}","{{item.Email}}")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -90,6 +101,22 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF0000FF"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
@@ -186,10 +213,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -205,15 +233,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF005696"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -262,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,9 +336,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -328,6 +371,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -503,28 +547,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="G1" s="10" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L1" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -538,25 +582,28 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -569,39 +616,43 @@
       <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="I5">
+      <c r="F5" s="11"/>
+      <c r="G5" s="3"/>
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>11</v>
       </c>
@@ -617,23 +668,23 @@
       <c r="E6">
         <v>15</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>16</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>17</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>12</v>
       </c>
@@ -649,23 +700,23 @@
       <c r="E7">
         <v>16</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>17</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>18</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>5</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>13</v>
       </c>
@@ -681,23 +732,23 @@
       <c r="E8">
         <v>17</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>19</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>6</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>7</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>14</v>
       </c>
@@ -713,23 +764,23 @@
       <c r="E9">
         <v>18</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>20</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>7</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>8</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>15</v>
       </c>
@@ -745,14 +796,14 @@
       <c r="E10">
         <v>19</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>20</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>16</v>
       </c>
@@ -768,16 +819,16 @@
       <c r="E11">
         <v>20</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>21</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added hyperlink examples (#234)
added hyperlink examples (#234)
</commit_message>
<xml_diff>
--- a/tests/Templates/4.xlsx
+++ b/tests/Templates/4.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\asr\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
@@ -10,16 +15,16 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dates">Лист1!$G$3</definedName>
-    <definedName name="PlanData">Лист1!$A$4:$H$5</definedName>
-    <definedName name="PlanData_Hours">Лист1!$G$4</definedName>
+    <definedName name="dates">Лист1!$H$3</definedName>
+    <definedName name="PlanData">Лист1!$A$4:$I$5</definedName>
+    <definedName name="PlanData_Hours">Лист1!$H$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -61,16 +66,22 @@
   </si>
   <si>
     <t>{{index+1}}</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>&amp;=HYPERLINK("mailto:{{item.Email}}","{{item.Email}}")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -90,6 +101,22 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF0000FF"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
@@ -186,10 +213,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -205,15 +233,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF005696"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -262,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,9 +336,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -328,6 +371,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -503,28 +547,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="G1" s="10" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L1" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -538,25 +582,28 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -569,39 +616,43 @@
       <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="I5">
+      <c r="F5" s="11"/>
+      <c r="G5" s="3"/>
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>11</v>
       </c>
@@ -617,23 +668,23 @@
       <c r="E6">
         <v>15</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>16</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>17</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>12</v>
       </c>
@@ -649,23 +700,23 @@
       <c r="E7">
         <v>16</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>17</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>18</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>5</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>13</v>
       </c>
@@ -681,23 +732,23 @@
       <c r="E8">
         <v>17</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>19</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>6</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>7</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>14</v>
       </c>
@@ -713,23 +764,23 @@
       <c r="E9">
         <v>18</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>20</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>7</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>8</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>15</v>
       </c>
@@ -745,14 +796,14 @@
       <c r="E10">
         <v>19</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>20</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>16</v>
       </c>
@@ -768,16 +819,16 @@
       <c r="E11">
         <v>20</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>21</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>